<commit_message>
script sincronização alocacao , horas planejadas e projeto ok
</commit_message>
<xml_diff>
--- a/scripts/excel/SGI Cloud & DevOps.xlsx
+++ b/scripts/excel/SGI Cloud & DevOps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://weg365.sharepoint.com/teams/BR-TI-SGI/Recursos em projetos/SGI - Detalhamento Atividades/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A807F7CC-2422-4A1E-B36D-EF0FF3F005BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{655EC8AC-3B50-4C19-BE63-575F68136F14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="4" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="16" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="132">
   <si>
     <t>Epic</t>
   </si>
@@ -226,6 +226,9 @@
   </si>
   <si>
     <t>DTI_XX (Tarefa Administrativa, Rotina, Treinamento, ...)</t>
+  </si>
+  <si>
+    <t>dsfsfsdfsdfsdf</t>
   </si>
   <si>
     <t>Em andamento</t>
@@ -6000,9 +6003,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C75895F1-0B30-415F-A22E-3A02614B8C8B}">
   <dimension ref="A1:AE18"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L1" sqref="L1:M1048576"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6496,18 +6499,21 @@
       <c r="AD6" s="41"/>
       <c r="AE6" s="41"/>
     </row>
-    <row r="7" spans="1:31" ht="30">
+    <row r="7" spans="1:31" ht="30.75">
       <c r="A7" s="1" t="s">
         <v>53</v>
       </c>
+      <c r="B7" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="C7" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F7" s="30">
         <v>406</v>
@@ -6591,16 +6597,16 @@
     </row>
     <row r="8" spans="1:31" ht="19.5" customHeight="1">
       <c r="A8" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D8" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="F8" s="29"/>
       <c r="G8" s="10">
@@ -6680,7 +6686,7 @@
     </row>
     <row r="9" spans="1:31" ht="19.5" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D9" s="22"/>
       <c r="F9" s="29"/>
@@ -6763,16 +6769,16 @@
     </row>
     <row r="10" spans="1:31">
       <c r="A10" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G10" s="10">
         <f t="shared" si="0"/>
@@ -6853,16 +6859,16 @@
     </row>
     <row r="11" spans="1:31">
       <c r="A11" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G11" s="10">
         <f t="shared" si="0"/>
@@ -6943,16 +6949,16 @@
     </row>
     <row r="12" spans="1:31">
       <c r="A12" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G12" s="10">
         <f t="shared" si="0"/>
@@ -7349,13 +7355,13 @@
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="K1" s="36" t="s">
         <v>28</v>
@@ -7831,10 +7837,10 @@
         <v>53</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>26</v>
@@ -7928,13 +7934,13 @@
     </row>
     <row r="8" spans="1:34">
       <c r="A8" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="22" t="s">
         <v>66</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D8" s="22" t="s">
-        <v>65</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>26</v>
@@ -8028,16 +8034,16 @@
     </row>
     <row r="9" spans="1:34" ht="30" hidden="1">
       <c r="A9" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>26</v>
@@ -8109,13 +8115,13 @@
     </row>
     <row r="10" spans="1:34">
       <c r="A10" s="14" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>26</v>
@@ -8199,13 +8205,13 @@
     </row>
     <row r="11" spans="1:34">
       <c r="A11" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>26</v>
@@ -8285,16 +8291,16 @@
     </row>
     <row r="12" spans="1:34" ht="15.75" customHeight="1">
       <c r="A12" s="59" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>26</v>
@@ -8376,16 +8382,16 @@
     </row>
     <row r="13" spans="1:34">
       <c r="A13" s="59" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>26</v>
@@ -8467,16 +8473,16 @@
     </row>
     <row r="14" spans="1:34">
       <c r="A14" s="59" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="C14" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>26</v>
@@ -8570,13 +8576,13 @@
     </row>
     <row r="15" spans="1:34" hidden="1">
       <c r="A15" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>26</v>
@@ -8672,13 +8678,13 @@
     </row>
     <row r="16" spans="1:34" hidden="1">
       <c r="A16" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>26</v>
@@ -8750,14 +8756,14 @@
     </row>
     <row r="17" spans="1:34">
       <c r="A17" s="60" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B17" s="25"/>
       <c r="C17" s="12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>26</v>
@@ -8853,11 +8859,11 @@
     </row>
     <row r="18" spans="1:34" hidden="1">
       <c r="A18" s="26" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B18" s="25"/>
       <c r="C18" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D18" s="1">
         <v>2024</v>
@@ -8932,11 +8938,11 @@
     </row>
     <row r="19" spans="1:34" hidden="1">
       <c r="A19" s="26" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B19" s="25"/>
       <c r="C19" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D19" s="1">
         <v>2024</v>
@@ -9011,10 +9017,10 @@
     </row>
     <row r="20" spans="1:34" hidden="1">
       <c r="A20" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D20" s="1">
         <v>2024</v>
@@ -9089,14 +9095,14 @@
     </row>
     <row r="21" spans="1:34">
       <c r="A21" s="26" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B21" s="25"/>
       <c r="C21" s="12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>26</v>
@@ -9192,16 +9198,16 @@
     </row>
     <row r="22" spans="1:34" hidden="1">
       <c r="A22" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D22" s="22" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>26</v>
@@ -9297,10 +9303,10 @@
     </row>
     <row r="23" spans="1:34" hidden="1">
       <c r="A23" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D23" s="1">
         <v>2024</v>
@@ -9375,10 +9381,10 @@
     </row>
     <row r="24" spans="1:34" hidden="1">
       <c r="A24" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D24" s="1">
         <v>2024</v>
@@ -9453,10 +9459,10 @@
     </row>
     <row r="25" spans="1:34" hidden="1">
       <c r="A25" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D25" s="1">
         <v>2024</v>
@@ -9531,10 +9537,10 @@
     </row>
     <row r="26" spans="1:34" hidden="1">
       <c r="A26" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D26" s="1">
         <v>2024</v>
@@ -9609,13 +9615,13 @@
     </row>
     <row r="27" spans="1:34">
       <c r="A27" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D27" s="22" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>26</v>
@@ -9711,10 +9717,10 @@
     </row>
     <row r="28" spans="1:34" hidden="1">
       <c r="A28" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D28" s="1">
         <v>2024</v>
@@ -9789,13 +9795,13 @@
     </row>
     <row r="29" spans="1:34" hidden="1">
       <c r="A29" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>26</v>
@@ -9891,10 +9897,10 @@
     </row>
     <row r="30" spans="1:34" ht="30" hidden="1">
       <c r="A30" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D30" s="1">
         <v>2024</v>
@@ -9969,10 +9975,10 @@
     </row>
     <row r="31" spans="1:34" hidden="1">
       <c r="A31" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D31" s="1">
         <v>2024</v>
@@ -10047,10 +10053,10 @@
     </row>
     <row r="32" spans="1:34" hidden="1">
       <c r="A32" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D32" s="1">
         <v>2024</v>
@@ -10125,10 +10131,10 @@
     </row>
     <row r="33" spans="1:34" hidden="1">
       <c r="A33" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D33" s="1">
         <v>2024</v>
@@ -10203,10 +10209,10 @@
     </row>
     <row r="34" spans="1:34" hidden="1">
       <c r="A34" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D34" s="1">
         <v>2024</v>
@@ -10281,13 +10287,13 @@
     </row>
     <row r="35" spans="1:34" hidden="1">
       <c r="A35" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D35" s="22" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>26</v>
@@ -10383,13 +10389,13 @@
     </row>
     <row r="36" spans="1:34" hidden="1">
       <c r="A36" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D36" s="22" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>26</v>
@@ -10461,13 +10467,13 @@
     </row>
     <row r="37" spans="1:34" hidden="1">
       <c r="A37" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D37" s="22" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>26</v>
@@ -10563,16 +10569,16 @@
     </row>
     <row r="38" spans="1:34">
       <c r="A38" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D38" s="22" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>26</v>
@@ -10662,13 +10668,13 @@
     </row>
     <row r="39" spans="1:34">
       <c r="A39" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D39" s="22" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>26</v>
@@ -10762,7 +10768,7 @@
     </row>
     <row r="40" spans="1:34">
       <c r="A40" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B40" s="1">
         <v>2026</v>
@@ -10865,7 +10871,7 @@
     </row>
     <row r="41" spans="1:34">
       <c r="A41" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B41" s="1">
         <v>2026</v>
@@ -10971,7 +10977,7 @@
         <v>24</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D42" s="1">
         <v>2025</v>
@@ -11068,13 +11074,13 @@
     </row>
     <row r="43" spans="1:34" ht="30" hidden="1">
       <c r="A43" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D43" s="1">
         <v>2025</v>
@@ -11171,13 +11177,13 @@
     </row>
     <row r="44" spans="1:34" ht="30" hidden="1">
       <c r="A44" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>104</v>
-      </c>
       <c r="C44" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D44" s="1">
         <v>2025</v>
@@ -11274,13 +11280,13 @@
     </row>
     <row r="45" spans="1:34" ht="30" hidden="1">
       <c r="A45" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D45" s="1">
         <v>2025</v>
@@ -11377,13 +11383,13 @@
     </row>
     <row r="46" spans="1:34" ht="30" hidden="1">
       <c r="A46" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D46" s="1">
         <v>2025</v>
@@ -11480,13 +11486,13 @@
     </row>
     <row r="47" spans="1:34">
       <c r="A47" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D47" s="22" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>26</v>
@@ -11580,13 +11586,13 @@
     </row>
     <row r="48" spans="1:34">
       <c r="A48" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D48" s="22" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>26</v>
@@ -11680,16 +11686,16 @@
     </row>
     <row r="49" spans="1:34">
       <c r="A49" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B49" s="58" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D49" s="22" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>26</v>
@@ -11779,13 +11785,13 @@
     </row>
     <row r="50" spans="1:34" hidden="1">
       <c r="A50" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D50" s="22" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>26</v>
@@ -11875,13 +11881,13 @@
     </row>
     <row r="51" spans="1:34">
       <c r="A51" s="59" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D51" s="22" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>26</v>
@@ -11980,13 +11986,13 @@
     </row>
     <row r="52" spans="1:34">
       <c r="A52" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D52" s="22" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>26</v>
@@ -12076,13 +12082,13 @@
     </row>
     <row r="53" spans="1:34" hidden="1">
       <c r="A53" s="9" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D53" s="22" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>26</v>
@@ -12172,13 +12178,13 @@
     </row>
     <row r="54" spans="1:34" hidden="1">
       <c r="A54" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D54" s="22" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>26</v>
@@ -12268,13 +12274,13 @@
     </row>
     <row r="55" spans="1:34">
       <c r="A55" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D55" s="22" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>26</v>
@@ -12362,13 +12368,13 @@
     </row>
     <row r="56" spans="1:34">
       <c r="A56" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D56" s="22" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>26</v>
@@ -12454,13 +12460,13 @@
     </row>
     <row r="57" spans="1:34">
       <c r="A57" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D57" s="22" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>26</v>
@@ -12544,16 +12550,16 @@
     </row>
     <row r="58" spans="1:34">
       <c r="A58" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D58" s="22" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>26</v>
@@ -12637,16 +12643,16 @@
     </row>
     <row r="59" spans="1:34">
       <c r="A59" s="59" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D59" s="22" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>26</v>
@@ -12728,13 +12734,13 @@
     </row>
     <row r="60" spans="1:34">
       <c r="A60" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D60" s="22" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>26</v>
@@ -12998,7 +13004,7 @@
   <sheetData>
     <row r="1" spans="1:23">
       <c r="B1" s="43" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C1" s="43" t="s">
         <v>31</v>
@@ -13066,7 +13072,7 @@
     </row>
     <row r="2" spans="1:23">
       <c r="A2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:23">
@@ -13164,7 +13170,7 @@
     </row>
     <row r="4" spans="1:23">
       <c r="A4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B4" s="34">
         <f>'Ricardo K'!M3</f>
@@ -13257,7 +13263,7 @@
     </row>
     <row r="5" spans="1:23">
       <c r="A5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B5" s="34">
         <f>'Ricardo K'!M4</f>
@@ -13364,7 +13370,7 @@
     </row>
     <row r="7" spans="1:23">
       <c r="A7" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:23">
@@ -13462,7 +13468,7 @@
     </row>
     <row r="9" spans="1:23">
       <c r="A9" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B9" s="34">
         <f>'João Vitor'!J3</f>
@@ -13555,7 +13561,7 @@
     </row>
     <row r="10" spans="1:23">
       <c r="A10" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B10" s="34">
         <f>'João Vitor'!J4</f>
@@ -13655,7 +13661,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BD7975B-B404-4214-A6EF-2AB2EC0EBBE6}">
   <dimension ref="A1:W48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="N46" sqref="N46:O48"/>
     </sheetView>
   </sheetViews>
@@ -13671,7 +13677,7 @@
   <sheetData>
     <row r="1" spans="1:23">
       <c r="B1" s="43" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C1" s="43" t="s">
         <v>31</v>
@@ -13739,7 +13745,7 @@
     </row>
     <row r="2" spans="1:23">
       <c r="A2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B2" s="50"/>
       <c r="C2" s="50"/>
@@ -13766,12 +13772,12 @@
     </row>
     <row r="3" spans="1:23">
       <c r="A3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:23">
       <c r="A4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B4" s="34">
         <f>('Ricardo K'!M3)*0.3</f>
@@ -13864,7 +13870,7 @@
     </row>
     <row r="5" spans="1:23">
       <c r="A5" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B5" s="46">
         <f>171*0.3</f>
@@ -13917,12 +13923,12 @@
     </row>
     <row r="7" spans="1:23">
       <c r="A7" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:23">
       <c r="A8" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B8" s="34">
         <f>('João Vitor'!J3)*0.8</f>
@@ -14015,7 +14021,7 @@
     </row>
     <row r="9" spans="1:23">
       <c r="A9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B9" s="46">
         <f>168*0.8</f>
@@ -14054,7 +14060,7 @@
     </row>
     <row r="12" spans="1:23">
       <c r="A12" s="48" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B12" s="49">
         <v>45717</v>
@@ -14071,7 +14077,7 @@
     </row>
     <row r="13" spans="1:23">
       <c r="A13" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B13" s="34">
         <f>SUM(B4,B8)</f>
@@ -14164,7 +14170,7 @@
     </row>
     <row r="14" spans="1:23">
       <c r="A14" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B14" s="46">
         <f>SUM(B5,B9)</f>
@@ -14203,17 +14209,17 @@
     </row>
     <row r="17" spans="1:23">
       <c r="A17" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="18" spans="1:23">
       <c r="A18" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:23">
       <c r="A19" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B19" s="52">
         <f>('Ricardo K'!M3)*0.7</f>
@@ -14306,7 +14312,7 @@
     </row>
     <row r="20" spans="1:23">
       <c r="A20" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B20" s="46">
         <f>171*0.7</f>
@@ -14359,12 +14365,12 @@
     </row>
     <row r="22" spans="1:23">
       <c r="A22" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="23" spans="1:23">
       <c r="A23" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B23" s="34">
         <f>('João Vitor'!J3)*0.2</f>
@@ -14457,7 +14463,7 @@
     </row>
     <row r="24" spans="1:23">
       <c r="A24" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B24" s="46">
         <f>168*0.2</f>
@@ -14496,7 +14502,7 @@
     </row>
     <row r="27" spans="1:23">
       <c r="A27" s="48" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B27" s="49">
         <v>45717</v>
@@ -14513,7 +14519,7 @@
     </row>
     <row r="28" spans="1:23">
       <c r="A28" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B28" s="34">
         <f>SUM(B19,B23)</f>
@@ -14606,7 +14612,7 @@
     </row>
     <row r="29" spans="1:23">
       <c r="A29" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B29" s="46">
         <f>SUM(B20,B24)</f>

</xml_diff>